<commit_message>
carga de trazas, mostly dumpear el working dir
</commit_message>
<xml_diff>
--- a/resources/templates/cape.xlsx
+++ b/resources/templates/cape.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Autoparte</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Aplicación</t>
   </si>
   <si>
-    <t>1.3.1</t>
-  </si>
-  <si>
     <t>4203.30.00</t>
   </si>
   <si>
@@ -71,6 +68,9 @@
   </si>
   <si>
     <t>Peso / Unidad</t>
+  </si>
+  <si>
+    <t>Familia</t>
   </si>
 </sst>
 </file>
@@ -195,10 +195,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -596,7 +597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -605,62 +606,66 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -676,7 +681,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -685,80 +690,83 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="3"/>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="1"/>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
+    <row r="4" spans="1:16">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
pictures en cape y exchas
</commit_message>
<xml_diff>
--- a/resources/templates/cape.xlsx
+++ b/resources/templates/cape.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Autoparte</t>
   </si>
@@ -71,13 +71,16 @@
   </si>
   <si>
     <t>Familia</t>
+  </si>
+  <si>
+    <t>Fotos (IF)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +111,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -117,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -125,6 +136,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -195,11 +251,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -597,7 +662,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -624,48 +689,51 @@
     <col min="17" max="17" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" ht="31" thickBot="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>